<commit_message>
chore: update pv pvc volumes
</commit_message>
<xml_diff>
--- a/variables.xlsx
+++ b/variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4a86ff3241b6be39/Documentos/TELNETSP/SUNAT MLOPS/Instalacion-configuracion-minikube/git-repo/mlops-sunat-config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{F990C88A-5093-4CF2-AA0D-BA0F37204D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6DE33B3D-55BB-4BDF-B5C5-5920513B5D53}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{F990C88A-5093-4CF2-AA0D-BA0F37204D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E89299F-9581-4D36-98E4-276127C80230}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{28FD25A8-6F2B-45A1-B52D-89D9B965DB76}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="129">
   <si>
     <t>quay.io/kuberay/operator</t>
   </si>
@@ -403,6 +403,15 @@
   </si>
   <si>
     <t>csi-driver-nfs-4.11.0-sunat.tgz</t>
+  </si>
+  <si>
+    <t>8Gi</t>
+  </si>
+  <si>
+    <t>90Gi</t>
+  </si>
+  <si>
+    <t>volumeSize</t>
   </si>
 </sst>
 </file>
@@ -755,10 +764,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D5897E1-0AF6-42B1-B4C3-C4220E7D9890}">
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D50" sqref="D2:D50"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -805,7 +814,7 @@
         <v>104</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D50" si="0">$A$1&amp;":"&amp;A3&amp;"|"&amp;$B$1&amp;":"&amp;B3&amp;"|"&amp;$C$1&amp;":"&amp;C3</f>
+        <f t="shared" ref="D3:D57" si="0">$A$1&amp;":"&amp;A3&amp;"|"&amp;$B$1&amp;":"&amp;B3&amp;"|"&amp;$C$1&amp;":"&amp;C3</f>
         <v>VARIABLE:mlflowImage|AKS:burakince/mlflow|SUNAT:vcf-np-w2-harbor-az1.sunat.peru/mlops/burakince/mlflow</v>
       </c>
     </row>
@@ -1512,6 +1521,21 @@
       <c r="D50" t="str">
         <f t="shared" si="0"/>
         <v>VARIABLE:csiDriverNfs|AKS:csi-driver-nfs-4.11.0.tgz|SUNAT:csi-driver-nfs-4.11.0-sunat.tgz</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>128</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D51" t="str">
+        <f t="shared" si="0"/>
+        <v>VARIABLE:volumeSize|AKS:8Gi|SUNAT:90Gi</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: update storageclassname dinamico
</commit_message>
<xml_diff>
--- a/variables.xlsx
+++ b/variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4a86ff3241b6be39/Documentos/TELNETSP/SUNAT MLOPS/Instalacion-configuracion-minikube/git-repo/mlops-sunat-config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="8_{F990C88A-5093-4CF2-AA0D-BA0F37204D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E89299F-9581-4D36-98E4-276127C80230}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="8_{F990C88A-5093-4CF2-AA0D-BA0F37204D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{47F98437-8F5B-4E54-9F50-98E2BC03CA05}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{28FD25A8-6F2B-45A1-B52D-89D9B965DB76}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="132">
   <si>
     <t>quay.io/kuberay/operator</t>
   </si>
@@ -412,6 +412,15 @@
   </si>
   <si>
     <t>volumeSize</t>
+  </si>
+  <si>
+    <t>storageClassName</t>
+  </si>
+  <si>
+    <t>storage-nfs</t>
+  </si>
+  <si>
+    <t>nfs-storage</t>
   </si>
 </sst>
 </file>
@@ -764,10 +773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D5897E1-0AF6-42B1-B4C3-C4220E7D9890}">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -814,7 +823,7 @@
         <v>104</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D57" si="0">$A$1&amp;":"&amp;A3&amp;"|"&amp;$B$1&amp;":"&amp;B3&amp;"|"&amp;$C$1&amp;":"&amp;C3</f>
+        <f t="shared" ref="D3:D52" si="0">$A$1&amp;":"&amp;A3&amp;"|"&amp;$B$1&amp;":"&amp;B3&amp;"|"&amp;$C$1&amp;":"&amp;C3</f>
         <v>VARIABLE:mlflowImage|AKS:burakince/mlflow|SUNAT:vcf-np-w2-harbor-az1.sunat.peru/mlops/burakince/mlflow</v>
       </c>
     </row>
@@ -1536,6 +1545,21 @@
       <c r="D51" t="str">
         <f t="shared" si="0"/>
         <v>VARIABLE:volumeSize|AKS:8Gi|SUNAT:90Gi</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>129</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D52" t="str">
+        <f t="shared" si="0"/>
+        <v>VARIABLE:storageClassName|AKS:nfs-storage|SUNAT:storage-nfs</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: replace images names static by variables
</commit_message>
<xml_diff>
--- a/variables.xlsx
+++ b/variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4a86ff3241b6be39/Documentos/TELNETSP/SUNAT MLOPS/Instalacion-configuracion-minikube/git-repo/mlops-sunat-config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="8_{F990C88A-5093-4CF2-AA0D-BA0F37204D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{47F98437-8F5B-4E54-9F50-98E2BC03CA05}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{77D53042-D86C-4942-91DB-ED37F83740C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{74FC747D-3133-40E5-997A-4EB5507CF5CE}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{28FD25A8-6F2B-45A1-B52D-89D9B965DB76}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="180">
   <si>
     <t>quay.io/kuberay/operator</t>
   </si>
@@ -408,19 +408,163 @@
     <t>8Gi</t>
   </si>
   <si>
-    <t>90Gi</t>
-  </si>
-  <si>
     <t>volumeSize</t>
   </si>
   <si>
     <t>storageClassName</t>
   </si>
   <si>
-    <t>storage-nfs</t>
-  </si>
-  <si>
     <t>nfs-storage</t>
+  </si>
+  <si>
+    <t>minioImageVersion</t>
+  </si>
+  <si>
+    <t>minioImageRepo</t>
+  </si>
+  <si>
+    <t>minioImageRegistry</t>
+  </si>
+  <si>
+    <t>docker.io</t>
+  </si>
+  <si>
+    <t>bitnami/jenkins</t>
+  </si>
+  <si>
+    <t>2.401.1-debian-11-r0</t>
+  </si>
+  <si>
+    <t>vcf-np-w2-harbor-az1.sunat.peru</t>
+  </si>
+  <si>
+    <t>rayserve/jenkins</t>
+  </si>
+  <si>
+    <t>latest</t>
+  </si>
+  <si>
+    <t>jenkinsImageRepo</t>
+  </si>
+  <si>
+    <t>jenkinsImageRegistry</t>
+  </si>
+  <si>
+    <t>jenkinsImageVersion</t>
+  </si>
+  <si>
+    <t>jenkinsAgentImageRepo</t>
+  </si>
+  <si>
+    <t>jenkinsAgentImageRegistry</t>
+  </si>
+  <si>
+    <t>jenkinsAgentImageVersion</t>
+  </si>
+  <si>
+    <t>bitnami/jenkins-agent</t>
+  </si>
+  <si>
+    <t>0.3107.0-debian-11-r36</t>
+  </si>
+  <si>
+    <t>rayserve/jenkins-agent</t>
+  </si>
+  <si>
+    <t>jenkinsInitContainerImage</t>
+  </si>
+  <si>
+    <t>busybox</t>
+  </si>
+  <si>
+    <t>vcf-np-w2-harbor-az1.sunat.peru/rayserve/busybox:latest</t>
+  </si>
+  <si>
+    <t>jenkinsShellImageRepo</t>
+  </si>
+  <si>
+    <t>jenkinsShellImageRegistry</t>
+  </si>
+  <si>
+    <t>jenkinsShellImageVersion</t>
+  </si>
+  <si>
+    <t>bitnami/bitnami-shell</t>
+  </si>
+  <si>
+    <t>11-debian-11-r126</t>
+  </si>
+  <si>
+    <t>rayserve/bitnami-shell</t>
+  </si>
+  <si>
+    <t>11-r38</t>
+  </si>
+  <si>
+    <t>bitnami/minio</t>
+  </si>
+  <si>
+    <t>2022.10.20-debian-11-r0</t>
+  </si>
+  <si>
+    <t>rayserve/minio</t>
+  </si>
+  <si>
+    <t>minioClientImageRegistry</t>
+  </si>
+  <si>
+    <t>minioClientImageRepo</t>
+  </si>
+  <si>
+    <t>minioClientImageVersion</t>
+  </si>
+  <si>
+    <t>bitnami/minio-client</t>
+  </si>
+  <si>
+    <t>2022.10.12-debian-11-r1</t>
+  </si>
+  <si>
+    <t>2022.10.6-debian-11-r1</t>
+  </si>
+  <si>
+    <t>11-debian-11-r43</t>
+  </si>
+  <si>
+    <t>minioShellImageRegistry</t>
+  </si>
+  <si>
+    <t>minioShellImageVersion</t>
+  </si>
+  <si>
+    <t>minioShellImageRepo</t>
+  </si>
+  <si>
+    <t>postgresJupyterhubImageRegistry</t>
+  </si>
+  <si>
+    <t>postgresJupyterhubImageRepo</t>
+  </si>
+  <si>
+    <t>postgresJupyterhubImageVersion</t>
+  </si>
+  <si>
+    <t>bitnami/postgresql</t>
+  </si>
+  <si>
+    <t>14.5.0-debian-11-r31</t>
+  </si>
+  <si>
+    <t>rayserve/postgresql</t>
+  </si>
+  <si>
+    <t>postgresImageRegistry</t>
+  </si>
+  <si>
+    <t>postgresImageRepo</t>
+  </si>
+  <si>
+    <t>postgresImageVersion</t>
   </si>
 </sst>
 </file>
@@ -474,6 +618,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -773,10 +921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D5897E1-0AF6-42B1-B4C3-C4220E7D9890}">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -823,7 +971,7 @@
         <v>104</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D52" si="0">$A$1&amp;":"&amp;A3&amp;"|"&amp;$B$1&amp;":"&amp;B3&amp;"|"&amp;$C$1&amp;":"&amp;C3</f>
+        <f t="shared" ref="D3:D62" si="0">$A$1&amp;":"&amp;A3&amp;"|"&amp;$B$1&amp;":"&amp;B3&amp;"|"&amp;$C$1&amp;":"&amp;C3</f>
         <v>VARIABLE:mlflowImage|AKS:burakince/mlflow|SUNAT:vcf-np-w2-harbor-az1.sunat.peru/mlops/burakince/mlflow</v>
       </c>
     </row>
@@ -1534,32 +1682,407 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>126</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D51" t="str">
         <f t="shared" si="0"/>
-        <v>VARIABLE:volumeSize|AKS:8Gi|SUNAT:90Gi</v>
+        <v>VARIABLE:volumeSize|AKS:8Gi|SUNAT:8Gi</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
+        <v>128</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="C52" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D52" t="str">
+        <f t="shared" si="0"/>
+        <v>VARIABLE:storageClassName|AKS:nfs-storage|SUNAT:nfs-storage</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>140</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D53" t="str">
+        <f t="shared" si="0"/>
+        <v>VARIABLE:jenkinsImageRegistry|AKS:docker.io|SUNAT:vcf-np-w2-harbor-az1.sunat.peru</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>139</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D54" t="str">
+        <f t="shared" si="0"/>
+        <v>VARIABLE:jenkinsImageRepo|AKS:bitnami/jenkins|SUNAT:rayserve/jenkins</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>141</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D55" t="str">
+        <f t="shared" si="0"/>
+        <v>VARIABLE:jenkinsImageVersion|AKS:2.401.1-debian-11-r0|SUNAT:latest</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>143</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D56" t="str">
+        <f t="shared" si="0"/>
+        <v>VARIABLE:jenkinsAgentImageRegistry|AKS:docker.io|SUNAT:vcf-np-w2-harbor-az1.sunat.peru</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>142</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D57" t="str">
+        <f t="shared" si="0"/>
+        <v>VARIABLE:jenkinsAgentImageRepo|AKS:bitnami/jenkins-agent|SUNAT:rayserve/jenkins-agent</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>144</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D58" t="str">
+        <f t="shared" si="0"/>
+        <v>VARIABLE:jenkinsAgentImageVersion|AKS:0.3107.0-debian-11-r36|SUNAT:latest</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>148</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D59" t="str">
+        <f t="shared" si="0"/>
+        <v>VARIABLE:jenkinsInitContainerImage|AKS:busybox|SUNAT:vcf-np-w2-harbor-az1.sunat.peru/rayserve/busybox:latest</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>152</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D60" t="str">
+        <f t="shared" si="0"/>
+        <v>VARIABLE:jenkinsShellImageRegistry|AKS:docker.io|SUNAT:vcf-np-w2-harbor-az1.sunat.peru</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>151</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D61" t="str">
+        <f t="shared" si="0"/>
+        <v>VARIABLE:jenkinsShellImageRepo|AKS:bitnami/bitnami-shell|SUNAT:rayserve/bitnami-shell</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>153</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D62" t="str">
+        <f t="shared" si="0"/>
+        <v>VARIABLE:jenkinsShellImageVersion|AKS:11-debian-11-r126|SUNAT:11-r38</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>132</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D63" t="str">
+        <f>$A$1&amp;":"&amp;A63&amp;"|"&amp;$B$1&amp;":"&amp;B63&amp;"|"&amp;$C$1&amp;":"&amp;C63</f>
+        <v>VARIABLE:minioImageRegistry|AKS:docker.io|SUNAT:vcf-np-w2-harbor-az1.sunat.peru</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
         <v>131</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="B64" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D64" t="str">
+        <f>$A$1&amp;":"&amp;A64&amp;"|"&amp;$B$1&amp;":"&amp;B64&amp;"|"&amp;$C$1&amp;":"&amp;C64</f>
+        <v>VARIABLE:minioImageRepo|AKS:bitnami/minio|SUNAT:rayserve/minio</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
         <v>130</v>
       </c>
-      <c r="D52" t="str">
-        <f t="shared" si="0"/>
-        <v>VARIABLE:storageClassName|AKS:nfs-storage|SUNAT:storage-nfs</v>
+      <c r="B65" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D65" t="str">
+        <f>$A$1&amp;":"&amp;A65&amp;"|"&amp;$B$1&amp;":"&amp;B65&amp;"|"&amp;$C$1&amp;":"&amp;C65</f>
+        <v>VARIABLE:minioImageVersion|AKS:2022.10.20-debian-11-r0|SUNAT:latest</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>161</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D66" t="str">
+        <f>$A$1&amp;":"&amp;A66&amp;"|"&amp;$B$1&amp;":"&amp;B66&amp;"|"&amp;$C$1&amp;":"&amp;C66</f>
+        <v>VARIABLE:minioClientImageRegistry|AKS:docker.io|SUNAT:vcf-np-w2-harbor-az1.sunat.peru</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>162</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D67" t="str">
+        <f>$A$1&amp;":"&amp;A67&amp;"|"&amp;$B$1&amp;":"&amp;B67&amp;"|"&amp;$C$1&amp;":"&amp;C67</f>
+        <v>VARIABLE:minioClientImageRepo|AKS:bitnami/minio-client|SUNAT:rayserve/minio</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>163</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D68" t="str">
+        <f>$A$1&amp;":"&amp;A68&amp;"|"&amp;$B$1&amp;":"&amp;B68&amp;"|"&amp;$C$1&amp;":"&amp;C68</f>
+        <v>VARIABLE:minioClientImageVersion|AKS:2022.10.12-debian-11-r1|SUNAT:2022.10.6-debian-11-r1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>168</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D69" t="str">
+        <f t="shared" ref="D69:D74" si="1">$A$1&amp;":"&amp;A69&amp;"|"&amp;$B$1&amp;":"&amp;B69&amp;"|"&amp;$C$1&amp;":"&amp;C69</f>
+        <v>VARIABLE:minioShellImageRegistry|AKS:docker.io|SUNAT:vcf-np-w2-harbor-az1.sunat.peru</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>170</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D70" t="str">
+        <f t="shared" si="1"/>
+        <v>VARIABLE:minioShellImageRepo|AKS:bitnami/bitnami-shell|SUNAT:rayserve/minio</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>169</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D71" t="str">
+        <f t="shared" si="1"/>
+        <v>VARIABLE:minioShellImageVersion|AKS:11-debian-11-r43|SUNAT:latest</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>171</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D72" t="str">
+        <f t="shared" si="1"/>
+        <v>VARIABLE:postgresJupyterhubImageRegistry|AKS:docker.io|SUNAT:vcf-np-w2-harbor-az1.sunat.peru</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>172</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D73" t="str">
+        <f t="shared" si="1"/>
+        <v>VARIABLE:postgresJupyterhubImageRepo|AKS:bitnami/postgresql|SUNAT:rayserve/postgresql</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>173</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D74" t="str">
+        <f t="shared" si="1"/>
+        <v>VARIABLE:postgresJupyterhubImageVersion|AKS:14.5.0-debian-11-r31|SUNAT:latest</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>177</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D75" t="str">
+        <f t="shared" ref="D75:D77" si="2">$A$1&amp;":"&amp;A75&amp;"|"&amp;$B$1&amp;":"&amp;B75&amp;"|"&amp;$C$1&amp;":"&amp;C75</f>
+        <v>VARIABLE:postgresImageRegistry|AKS:docker.io|SUNAT:vcf-np-w2-harbor-az1.sunat.peru</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>178</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D76" t="str">
+        <f t="shared" si="2"/>
+        <v>VARIABLE:postgresImageRepo|AKS:bitnami/postgresql|SUNAT:rayserve/postgresql</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>179</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D77" t="str">
+        <f t="shared" si="2"/>
+        <v>VARIABLE:postgresImageVersion|AKS:14.5.0-debian-11-r31|SUNAT:latest</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
delete outdated charts and update variables xlsx
</commit_message>
<xml_diff>
--- a/variables.xlsx
+++ b/variables.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4a86ff3241b6be39/Documentos/TELNETSP/SUNAT MLOPS/Instalacion-configuracion-minikube/git-repo/mlops-sunat-config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{77D53042-D86C-4942-91DB-ED37F83740C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{74FC747D-3133-40E5-997A-4EB5507CF5CE}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{77D53042-D86C-4942-91DB-ED37F83740C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E4C5E2D1-CB25-4678-AE0A-EEF936138565}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{28FD25A8-6F2B-45A1-B52D-89D9B965DB76}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="183">
   <si>
     <t>quay.io/kuberay/operator</t>
   </si>
@@ -42,9 +43,6 @@
     <t>miguelsff/ray</t>
   </si>
   <si>
-    <t>2.41.0-py311-sunat</t>
-  </si>
-  <si>
     <t>quay.io/jupyterhub/k8s-hub</t>
   </si>
   <si>
@@ -69,12 +67,6 @@
     <t>quay.io/jupyterhub/k8s-network-tools</t>
   </si>
   <si>
-    <t>miguelsff/k8s-singleuser-sample</t>
-  </si>
-  <si>
-    <t>3.3.8-py31111-sunat</t>
-  </si>
-  <si>
     <t>registry.k8s.io/kube-scheduler</t>
   </si>
   <si>
@@ -360,9 +352,6 @@
     <t>vcf-np-w2-harbor-az1.sunat.peru/mlops/jupyterhub/k8s-network-tools</t>
   </si>
   <si>
-    <t>vcf-np-w2-harbor-az1.sunat.peru/mlops/miguelsff/k8s-singleuser-sample</t>
-  </si>
-  <si>
     <t>vcf-np-w2-harbor-az1.sunat.peru/mlops/kube-scheduler/kube-scheduler</t>
   </si>
   <si>
@@ -565,6 +554,27 @@
   </si>
   <si>
     <t>postgresImageVersion</t>
+  </si>
+  <si>
+    <t>miguelsff/scipy-notebook</t>
+  </si>
+  <si>
+    <t>vcf-np-w2-harbor-az1.sunat.peru/mlops/miguelsff/scipy-notebook</t>
+  </si>
+  <si>
+    <t>2.41.0-py311-sunat-v2</t>
+  </si>
+  <si>
+    <t>python-3.11-sunat-v3</t>
+  </si>
+  <si>
+    <t>kubeletDir</t>
+  </si>
+  <si>
+    <t>/var/lib/kubelet</t>
+  </si>
+  <si>
+    <t>/var/vcap/data/kubelet</t>
   </si>
 </sst>
 </file>
@@ -921,10 +931,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D5897E1-0AF6-42B1-B4C3-C4220E7D9890}">
-  <dimension ref="A1:D77"/>
+  <dimension ref="A1:D78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="D77" sqref="D77:D78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -936,24 +946,24 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D2" t="str">
         <f>$A$1&amp;":"&amp;A2&amp;"|"&amp;$B$1&amp;":"&amp;B2&amp;"|"&amp;$C$1&amp;":"&amp;C2</f>
@@ -962,13 +972,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" ref="D3:D62" si="0">$A$1&amp;":"&amp;A3&amp;"|"&amp;$B$1&amp;":"&amp;B3&amp;"|"&amp;$C$1&amp;":"&amp;C3</f>
@@ -977,13 +987,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
@@ -992,13 +1002,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
@@ -1007,13 +1017,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
@@ -1022,13 +1032,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
@@ -1037,13 +1047,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
@@ -1052,13 +1062,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
@@ -1067,28 +1077,28 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>14</v>
+        <v>176</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>111</v>
+        <v>177</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
-        <v>VARIABLE:singleUserImage|AKS:miguelsff/k8s-singleuser-sample|SUNAT:vcf-np-w2-harbor-az1.sunat.peru/mlops/miguelsff/k8s-singleuser-sample</v>
+        <v>VARIABLE:singleUserImage|AKS:miguelsff/scipy-notebook|SUNAT:vcf-np-w2-harbor-az1.sunat.peru/mlops/miguelsff/scipy-notebook</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
@@ -1097,13 +1107,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
@@ -1112,13 +1122,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
@@ -1127,13 +1137,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
@@ -1142,13 +1152,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
@@ -1157,13 +1167,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
@@ -1172,13 +1182,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
@@ -1187,13 +1197,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
@@ -1202,13 +1212,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
@@ -1217,13 +1227,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
@@ -1232,7 +1242,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>1</v>
@@ -1247,7 +1257,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>3</v>
@@ -1262,28 +1272,28 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>5</v>
+        <v>178</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>5</v>
+        <v>178</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" si="0"/>
-        <v>VARIABLE:rayImageVersion|AKS:2.41.0-py311-sunat|SUNAT:2.41.0-py311-sunat</v>
+        <v>VARIABLE:rayImageVersion|AKS:2.41.0-py311-sunat-v2|SUNAT:2.41.0-py311-sunat-v2</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D24" t="str">
         <f t="shared" si="0"/>
@@ -1292,13 +1302,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D25" t="str">
         <f t="shared" si="0"/>
@@ -1307,13 +1317,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D26" t="str">
         <f t="shared" si="0"/>
@@ -1322,13 +1332,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D27" t="str">
         <f t="shared" si="0"/>
@@ -1337,13 +1347,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="0"/>
@@ -1352,28 +1362,28 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>15</v>
+        <v>179</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>15</v>
+        <v>179</v>
       </c>
       <c r="D29" t="str">
         <f t="shared" si="0"/>
-        <v>VARIABLE:singleUserImageVersion|AKS:3.3.8-py31111-sunat|SUNAT:3.3.8-py31111-sunat</v>
+        <v>VARIABLE:singleUserImageVersion|AKS:python-3.11-sunat-v3|SUNAT:python-3.11-sunat-v3</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D30" t="str">
         <f t="shared" si="0"/>
@@ -1382,7 +1392,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B31" s="1">
         <v>3.9</v>
@@ -1397,13 +1407,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D32" t="str">
         <f t="shared" si="0"/>
@@ -1412,13 +1422,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D33" t="str">
         <f t="shared" si="0"/>
@@ -1427,13 +1437,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D34" t="str">
         <f t="shared" si="0"/>
@@ -1442,13 +1452,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D35" t="str">
         <f t="shared" si="0"/>
@@ -1457,13 +1467,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D36" t="str">
         <f t="shared" si="0"/>
@@ -1472,13 +1482,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D37" t="str">
         <f t="shared" si="0"/>
@@ -1487,13 +1497,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D38" t="str">
         <f t="shared" si="0"/>
@@ -1502,13 +1512,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D39" t="str">
         <f t="shared" si="0"/>
@@ -1517,13 +1527,13 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D40" t="str">
         <f t="shared" si="0"/>
@@ -1532,13 +1542,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D41" t="str">
         <f t="shared" si="0"/>
@@ -1547,13 +1557,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D42" t="str">
         <f t="shared" si="0"/>
@@ -1562,13 +1572,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D43" t="str">
         <f t="shared" si="0"/>
@@ -1577,13 +1587,13 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D44" t="str">
         <f t="shared" si="0"/>
@@ -1592,13 +1602,13 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D45" t="str">
         <f t="shared" si="0"/>
@@ -1607,13 +1617,13 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D46" t="str">
         <f t="shared" si="0"/>
@@ -1622,13 +1632,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D47" t="str">
         <f t="shared" si="0"/>
@@ -1637,13 +1647,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
+        <v>68</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="D48" t="str">
         <f t="shared" si="0"/>
@@ -1652,13 +1662,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
+        <v>69</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="D49" t="str">
         <f t="shared" si="0"/>
@@ -1667,13 +1677,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D50" t="str">
         <f t="shared" si="0"/>
@@ -1682,13 +1692,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D51" t="str">
         <f t="shared" si="0"/>
@@ -1697,13 +1707,13 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D52" t="str">
         <f t="shared" si="0"/>
@@ -1712,13 +1722,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D53" t="str">
         <f t="shared" si="0"/>
@@ -1727,13 +1737,13 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D54" t="str">
         <f t="shared" si="0"/>
@@ -1742,13 +1752,13 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D55" t="str">
         <f t="shared" si="0"/>
@@ -1757,13 +1767,13 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D56" t="str">
         <f t="shared" si="0"/>
@@ -1772,13 +1782,13 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D57" t="str">
         <f t="shared" si="0"/>
@@ -1787,13 +1797,13 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D58" t="str">
         <f t="shared" si="0"/>
@@ -1802,13 +1812,13 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D59" t="str">
         <f t="shared" si="0"/>
@@ -1817,13 +1827,13 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D60" t="str">
         <f t="shared" si="0"/>
@@ -1832,13 +1842,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D61" t="str">
         <f t="shared" si="0"/>
@@ -1847,13 +1857,13 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
+        <v>149</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C62" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>157</v>
       </c>
       <c r="D62" t="str">
         <f t="shared" si="0"/>
@@ -1862,231 +1872,1113 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
+        <v>128</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C63" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B63" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>136</v>
-      </c>
       <c r="D63" t="str">
-        <f>$A$1&amp;":"&amp;A63&amp;"|"&amp;$B$1&amp;":"&amp;B63&amp;"|"&amp;$C$1&amp;":"&amp;C63</f>
+        <f t="shared" ref="D63:D68" si="1">$A$1&amp;":"&amp;A63&amp;"|"&amp;$B$1&amp;":"&amp;B63&amp;"|"&amp;$C$1&amp;":"&amp;C63</f>
         <v>VARIABLE:minioImageRegistry|AKS:docker.io|SUNAT:vcf-np-w2-harbor-az1.sunat.peru</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D64" t="str">
-        <f>$A$1&amp;":"&amp;A64&amp;"|"&amp;$B$1&amp;":"&amp;B64&amp;"|"&amp;$C$1&amp;":"&amp;C64</f>
+        <f t="shared" si="1"/>
         <v>VARIABLE:minioImageRepo|AKS:bitnami/minio|SUNAT:rayserve/minio</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D65" t="str">
-        <f>$A$1&amp;":"&amp;A65&amp;"|"&amp;$B$1&amp;":"&amp;B65&amp;"|"&amp;$C$1&amp;":"&amp;C65</f>
+        <f t="shared" si="1"/>
         <v>VARIABLE:minioImageVersion|AKS:2022.10.20-debian-11-r0|SUNAT:latest</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D66" t="str">
-        <f>$A$1&amp;":"&amp;A66&amp;"|"&amp;$B$1&amp;":"&amp;B66&amp;"|"&amp;$C$1&amp;":"&amp;C66</f>
+        <f t="shared" si="1"/>
         <v>VARIABLE:minioClientImageRegistry|AKS:docker.io|SUNAT:vcf-np-w2-harbor-az1.sunat.peru</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D67" t="str">
-        <f>$A$1&amp;":"&amp;A67&amp;"|"&amp;$B$1&amp;":"&amp;B67&amp;"|"&amp;$C$1&amp;":"&amp;C67</f>
+        <f t="shared" si="1"/>
         <v>VARIABLE:minioClientImageRepo|AKS:bitnami/minio-client|SUNAT:rayserve/minio</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D68" t="str">
-        <f>$A$1&amp;":"&amp;A68&amp;"|"&amp;$B$1&amp;":"&amp;B68&amp;"|"&amp;$C$1&amp;":"&amp;C68</f>
+        <f t="shared" si="1"/>
         <v>VARIABLE:minioClientImageVersion|AKS:2022.10.12-debian-11-r1|SUNAT:2022.10.6-debian-11-r1</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D69" t="str">
-        <f t="shared" ref="D69:D74" si="1">$A$1&amp;":"&amp;A69&amp;"|"&amp;$B$1&amp;":"&amp;B69&amp;"|"&amp;$C$1&amp;":"&amp;C69</f>
+        <f t="shared" ref="D69:D74" si="2">$A$1&amp;":"&amp;A69&amp;"|"&amp;$B$1&amp;":"&amp;B69&amp;"|"&amp;$C$1&amp;":"&amp;C69</f>
         <v>VARIABLE:minioShellImageRegistry|AKS:docker.io|SUNAT:vcf-np-w2-harbor-az1.sunat.peru</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D70" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>VARIABLE:minioShellImageRepo|AKS:bitnami/bitnami-shell|SUNAT:rayserve/minio</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D71" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>VARIABLE:minioShellImageVersion|AKS:11-debian-11-r43|SUNAT:latest</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D72" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>VARIABLE:postgresJupyterhubImageRegistry|AKS:docker.io|SUNAT:vcf-np-w2-harbor-az1.sunat.peru</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
+        <v>168</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C73" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B73" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>176</v>
-      </c>
       <c r="D73" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>VARIABLE:postgresJupyterhubImageRepo|AKS:bitnami/postgresql|SUNAT:rayserve/postgresql</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D74" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>VARIABLE:postgresJupyterhubImageVersion|AKS:14.5.0-debian-11-r31|SUNAT:latest</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D75" t="str">
-        <f t="shared" ref="D75:D77" si="2">$A$1&amp;":"&amp;A75&amp;"|"&amp;$B$1&amp;":"&amp;B75&amp;"|"&amp;$C$1&amp;":"&amp;C75</f>
+        <f t="shared" ref="D75:D78" si="3">$A$1&amp;":"&amp;A75&amp;"|"&amp;$B$1&amp;":"&amp;B75&amp;"|"&amp;$C$1&amp;":"&amp;C75</f>
         <v>VARIABLE:postgresImageRegistry|AKS:docker.io|SUNAT:vcf-np-w2-harbor-az1.sunat.peru</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D76" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>VARIABLE:postgresImageRepo|AKS:bitnami/postgresql|SUNAT:rayserve/postgresql</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D77" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>VARIABLE:postgresImageVersion|AKS:14.5.0-debian-11-r31|SUNAT:latest</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>180</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D78" t="str">
+        <f t="shared" si="3"/>
+        <v>VARIABLE:kubeletDir|AKS:/var/lib/kubelet|SUNAT:/var/vcap/data/kubelet</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A949FED9-021F-4DAC-9C1B-B76C98261044}">
+  <dimension ref="A1:C77"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C77"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="28.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="64.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" t="s">
+        <v>176</v>
+      </c>
+      <c r="C9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>83</v>
+      </c>
+      <c r="B22" t="s">
+        <v>178</v>
+      </c>
+      <c r="C22" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>84</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>85</v>
+      </c>
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>86</v>
+      </c>
+      <c r="B25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>87</v>
+      </c>
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>88</v>
+      </c>
+      <c r="B27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>89</v>
+      </c>
+      <c r="B28" t="s">
+        <v>179</v>
+      </c>
+      <c r="C28" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>90</v>
+      </c>
+      <c r="B29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>91</v>
+      </c>
+      <c r="B30">
+        <v>3.9</v>
+      </c>
+      <c r="C30">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>92</v>
+      </c>
+      <c r="B31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>93</v>
+      </c>
+      <c r="B32" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>94</v>
+      </c>
+      <c r="B33" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>95</v>
+      </c>
+      <c r="B34" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>96</v>
+      </c>
+      <c r="B35" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>97</v>
+      </c>
+      <c r="B36" t="s">
+        <v>26</v>
+      </c>
+      <c r="C36" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>98</v>
+      </c>
+      <c r="B37" t="s">
+        <v>28</v>
+      </c>
+      <c r="C37" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>99</v>
+      </c>
+      <c r="B38" t="s">
+        <v>24</v>
+      </c>
+      <c r="C38" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>60</v>
+      </c>
+      <c r="B39" t="s">
+        <v>32</v>
+      </c>
+      <c r="C39" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>61</v>
+      </c>
+      <c r="B40" t="s">
+        <v>33</v>
+      </c>
+      <c r="C40" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>62</v>
+      </c>
+      <c r="B41" t="s">
+        <v>34</v>
+      </c>
+      <c r="C41" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>63</v>
+      </c>
+      <c r="B42" t="s">
+        <v>35</v>
+      </c>
+      <c r="C42" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>64</v>
+      </c>
+      <c r="B43" t="s">
+        <v>36</v>
+      </c>
+      <c r="C43" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>65</v>
+      </c>
+      <c r="B44" t="s">
+        <v>37</v>
+      </c>
+      <c r="C44" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>66</v>
+      </c>
+      <c r="B45" t="s">
+        <v>38</v>
+      </c>
+      <c r="C45" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>67</v>
+      </c>
+      <c r="B46" t="s">
+        <v>39</v>
+      </c>
+      <c r="C46" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>68</v>
+      </c>
+      <c r="B47" t="s">
+        <v>40</v>
+      </c>
+      <c r="C47" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>69</v>
+      </c>
+      <c r="B48" t="s">
+        <v>41</v>
+      </c>
+      <c r="C48" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>119</v>
+      </c>
+      <c r="B49" t="s">
+        <v>120</v>
+      </c>
+      <c r="C49" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>123</v>
+      </c>
+      <c r="B50" t="s">
+        <v>122</v>
+      </c>
+      <c r="C50" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>124</v>
+      </c>
+      <c r="B51" t="s">
+        <v>125</v>
+      </c>
+      <c r="C51" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>136</v>
+      </c>
+      <c r="B52" t="s">
+        <v>129</v>
+      </c>
+      <c r="C52" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>135</v>
+      </c>
+      <c r="B53" t="s">
+        <v>130</v>
+      </c>
+      <c r="C53" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>137</v>
+      </c>
+      <c r="B54" t="s">
+        <v>131</v>
+      </c>
+      <c r="C54" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>139</v>
+      </c>
+      <c r="B55" t="s">
+        <v>129</v>
+      </c>
+      <c r="C55" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>138</v>
+      </c>
+      <c r="B56" t="s">
+        <v>141</v>
+      </c>
+      <c r="C56" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>140</v>
+      </c>
+      <c r="B57" t="s">
+        <v>142</v>
+      </c>
+      <c r="C57" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>144</v>
+      </c>
+      <c r="B58" t="s">
+        <v>145</v>
+      </c>
+      <c r="C58" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>148</v>
+      </c>
+      <c r="B59" t="s">
+        <v>129</v>
+      </c>
+      <c r="C59" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>147</v>
+      </c>
+      <c r="B60" t="s">
+        <v>150</v>
+      </c>
+      <c r="C60" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>149</v>
+      </c>
+      <c r="B61" t="s">
+        <v>151</v>
+      </c>
+      <c r="C61" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>128</v>
+      </c>
+      <c r="B62" t="s">
+        <v>129</v>
+      </c>
+      <c r="C62" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>127</v>
+      </c>
+      <c r="B63" t="s">
+        <v>154</v>
+      </c>
+      <c r="C63" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>126</v>
+      </c>
+      <c r="B64" t="s">
+        <v>155</v>
+      </c>
+      <c r="C64" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>157</v>
+      </c>
+      <c r="B65" t="s">
+        <v>129</v>
+      </c>
+      <c r="C65" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>158</v>
+      </c>
+      <c r="B66" t="s">
+        <v>160</v>
+      </c>
+      <c r="C66" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>159</v>
+      </c>
+      <c r="B67" t="s">
+        <v>161</v>
+      </c>
+      <c r="C67" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>164</v>
+      </c>
+      <c r="B68" t="s">
+        <v>129</v>
+      </c>
+      <c r="C68" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>166</v>
+      </c>
+      <c r="B69" t="s">
+        <v>150</v>
+      </c>
+      <c r="C69" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>165</v>
+      </c>
+      <c r="B70" t="s">
+        <v>163</v>
+      </c>
+      <c r="C70" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>167</v>
+      </c>
+      <c r="B71" t="s">
+        <v>129</v>
+      </c>
+      <c r="C71" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>168</v>
+      </c>
+      <c r="B72" t="s">
+        <v>170</v>
+      </c>
+      <c r="C72" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>169</v>
+      </c>
+      <c r="B73" t="s">
+        <v>171</v>
+      </c>
+      <c r="C73" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>173</v>
+      </c>
+      <c r="B74" t="s">
+        <v>129</v>
+      </c>
+      <c r="C74" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>174</v>
+      </c>
+      <c r="B75" t="s">
+        <v>170</v>
+      </c>
+      <c r="C75" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>175</v>
+      </c>
+      <c r="B76" t="s">
+        <v>171</v>
+      </c>
+      <c r="C76" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>180</v>
+      </c>
+      <c r="B77" t="s">
+        <v>181</v>
+      </c>
+      <c r="C77" t="s">
+        <v>182</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>